<commit_message>
fixing readability of markdowns
</commit_message>
<xml_diff>
--- a/tocheck/FloradePanama_dec4_2025_codigosperdidos.xlsx
+++ b/tocheck/FloradePanama_dec4_2025_codigosperdidos.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -655,7 +655,7 @@
         </is>
       </c>
       <c r="AD2" s="2">
-        <v>46057</v>
+        <v>46058</v>
       </c>
     </row>
   </sheetData>

</xml_diff>